<commit_message>
gpio and lcd descriptions added
</commit_message>
<xml_diff>
--- a/pcb/v1.1/power_consumption.xlsx
+++ b/pcb/v1.1/power_consumption.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Потребитель</t>
   </si>
@@ -39,9 +39,6 @@
     <t>NB3N501DG</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>PCF8547</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>TDA2003V</t>
+  </si>
+  <si>
+    <t>Примечание</t>
+  </si>
+  <si>
+    <t>U вых max = 6 В, U вых сред.кв = 5 В, R = 4 Ом =&gt; P = 6 Вт . КПД ~= 50%, потребление около 12 Вт =&gt; ток 1 А по 14.4 В</t>
   </si>
 </sst>
 </file>
@@ -148,9 +151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -169,6 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -466,37 +467,39 @@
   <dimension ref="B1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="127.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="60.75" customHeight="1" thickBot="1">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>3.8</v>
       </c>
       <c r="D2" s="2">
@@ -526,7 +529,7 @@
     </row>
     <row r="4" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>3.3</v>
@@ -542,7 +545,7 @@
     </row>
     <row r="5" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <v>3.8</v>
@@ -613,16 +616,18 @@
     </row>
     <row r="10" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
         <v>14.4</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
+      <c r="D10" s="5">
+        <v>1</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B11" s="1"/>
@@ -633,7 +638,7 @@
     </row>
     <row r="12" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -649,7 +654,7 @@
     </row>
     <row r="13" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -672,7 +677,7 @@
     </row>
     <row r="15" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <v>3.3</v>
@@ -695,7 +700,7 @@
     </row>
     <row r="17" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <v>4.2</v>
@@ -713,15 +718,15 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="9" t="s">
-        <v>16</v>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -729,7 +734,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f>SUM(E2:E17)</f>
         <v>10.825533</v>
       </c>
@@ -739,56 +744,56 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="2:6" ht="18" customHeight="1" thickBot="1">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
   </sheetData>

</xml_diff>